<commit_message>
fix(actions): fix github actions to work as intended, unit tests now pass and can be extended for BS forumlation
</commit_message>
<xml_diff>
--- a/tests/conf.xlsx
+++ b/tests/conf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BB11ED-8006-41F8-BBC3-03378C723BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6955EFC5-C45E-4E0D-9E47-0F9D1E886967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$78:$C$99</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="269">
   <si>
     <t>Default value</t>
   </si>
@@ -89,9 +89,6 @@
     <t>LV</t>
   </si>
   <si>
-    <t>LT</t>
-  </si>
-  <si>
     <t>LU</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>Path</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Hour 0 of the day is defined as midnight in timezone UTC+1</t>
   </si>
   <si>
@@ -398,9 +392,6 @@
     <t>OTH</t>
   </si>
   <si>
-    <t>Participation to reserve markets</t>
-  </si>
-  <si>
     <t>Price of Nuclear</t>
   </si>
   <si>
@@ -431,9 +422,6 @@
     <t>CPLEX path</t>
   </si>
   <si>
-    <t>Heat Demand</t>
-  </si>
-  <si>
     <t>Integer clustering</t>
   </si>
   <si>
@@ -470,9 +458,6 @@
     <t>Zonal</t>
   </si>
   <si>
-    <t>Price of Spillage</t>
-  </si>
-  <si>
     <t>Price of Unserved Heat</t>
   </si>
   <si>
@@ -590,9 +575,6 @@
     <t>Dummy configuration file for testing purposes. Two fictitious zones (Z1 and Z2) are simulated. The simulated period is only 7 days. There is a CHP unit in zone 1</t>
   </si>
   <si>
-    <t>Simulations/simulation_test</t>
-  </si>
-  <si>
     <t>tests/dummy_data/Load_RealTime/##/2015.csv</t>
   </si>
   <si>
@@ -602,9 +584,6 @@
     <t>tests/dummy_data/NTCs.csv</t>
   </si>
   <si>
-    <t>tests/dummy_data/CrossBorderFlows.csv</t>
-  </si>
-  <si>
     <t>Database/FuelPrices/Coal/2015.csv</t>
   </si>
   <si>
@@ -617,12 +596,6 @@
     <t>Database/FuelPrices/Biomass/2015.csv</t>
   </si>
   <si>
-    <t>tests/dummy_data/ReservoirLevels.csv</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/HeatDemand.csv</t>
-  </si>
-  <si>
     <t>tests/dummy_data/PriceOfPeat.csv</t>
   </si>
   <si>
@@ -635,106 +608,238 @@
     <t>Temperatures</t>
   </si>
   <si>
+    <t>Prices</t>
+  </si>
+  <si>
+    <t>Flexible Demand</t>
+  </si>
+  <si>
+    <t>The path is an absolute path or a relative path to this config file</t>
+  </si>
+  <si>
+    <t>This value imposes the final (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t>This value imposes the inital (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t>Value of lost load  in EUR/MWh</t>
+  </si>
+  <si>
+    <t>Time step in the data</t>
+  </si>
+  <si>
+    <t>Simulation time step</t>
+  </si>
+  <si>
+    <t>Number of hours</t>
+  </si>
+  <si>
+    <t>Share of quick start</t>
+  </si>
+  <si>
+    <t>Share of the 2U reserve that can be covered by quick start units</t>
+  </si>
+  <si>
+    <t>Demand flexibility</t>
+  </si>
+  <si>
+    <t>Number of equivalent storage hours for the flexibile demand</t>
+  </si>
+  <si>
+    <t>End of the Config file. This must be line number 325!</t>
+  </si>
+  <si>
+    <t>Price of Transmission</t>
+  </si>
+  <si>
+    <t>Price related to the usage of tranmission lines (in €/MWh)</t>
+  </si>
+  <si>
+    <t>Reserves Down</t>
+  </si>
+  <si>
+    <t>Reserves Up</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Geo_Coordinates.csv</t>
+  </si>
+  <si>
+    <t>ZZ3</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Probabilistic</t>
+  </si>
+  <si>
+    <t>Exogenous</t>
+  </si>
+  <si>
+    <t>Participation to reserve markets (CHP units)</t>
+  </si>
+  <si>
+    <t>Participation to reserve markets (Non-CHP units)</t>
+  </si>
+  <si>
+    <t>P2HT</t>
+  </si>
+  <si>
+    <t>ABHP</t>
+  </si>
+  <si>
+    <t>ASHP</t>
+  </si>
+  <si>
+    <t>GSHP</t>
+  </si>
+  <si>
+    <t>HYHP</t>
+  </si>
+  <si>
+    <t>WSHP</t>
+  </si>
+  <si>
+    <t>REHE</t>
+  </si>
+  <si>
+    <t>ALKE</t>
+  </si>
+  <si>
+    <t>PEME</t>
+  </si>
+  <si>
+    <t>SOXE</t>
+  </si>
+  <si>
+    <t>PEFC</t>
+  </si>
+  <si>
+    <t>DMFC</t>
+  </si>
+  <si>
+    <t>ALFC</t>
+  </si>
+  <si>
+    <t>PAFC</t>
+  </si>
+  <si>
+    <t>MCFC</t>
+  </si>
+  <si>
+    <t>SCSP</t>
+  </si>
+  <si>
+    <t>SOFC</t>
+  </si>
+  <si>
+    <t>REFC</t>
+  </si>
+  <si>
+    <t>Curtailment Cost</t>
+  </si>
+  <si>
+    <t>Price of Ammonia</t>
+  </si>
+  <si>
+    <t>Simulations/simulation_test_bs</t>
+  </si>
+  <si>
+    <t>Dispa-SET Configuration File (v20.03)</t>
+  </si>
+  <si>
+    <t>Boundary Sector Demand</t>
+  </si>
+  <si>
+    <t>Boundary Sector Inputs</t>
+  </si>
+  <si>
+    <t>Boundary Sector NTC</t>
+  </si>
+  <si>
+    <t>Boundary Sector Historical Flows</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_NTCs.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_CBFs.csv</t>
+  </si>
+  <si>
+    <t>Boundary Sector Demand (flexible)</t>
+  </si>
+  <si>
+    <t>GeoData (geographical coordinates)</t>
+  </si>
+  <si>
+    <t>Price of Userved Energy in the Boundary Sector</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Demand.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Inputs.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_FlexibleDemand.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Units_testcase.csv</t>
+  </si>
+  <si>
     <t>tests/dummy_data/Temperatures.csv</t>
   </si>
   <si>
-    <t>Prices</t>
-  </si>
-  <si>
-    <t>Flexible Demand</t>
-  </si>
-  <si>
-    <t>The path is an absolute path or a relative path to this config file</t>
-  </si>
-  <si>
-    <t>This value imposes the final (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t>This value imposes the inital (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t>Value of lost load  in EUR/MWh</t>
-  </si>
-  <si>
-    <t>Time step in the data</t>
-  </si>
-  <si>
-    <t>Simulation time step</t>
-  </si>
-  <si>
-    <t>Number of hours</t>
-  </si>
-  <si>
-    <t>Share of quick start</t>
-  </si>
-  <si>
-    <t>Share of the 2U reserve that can be covered by quick start units</t>
-  </si>
-  <si>
-    <t>Demand flexibility</t>
-  </si>
-  <si>
-    <t>Number of equivalent storage hours for the flexibile demand</t>
-  </si>
-  <si>
-    <t>End of the Config file. This must be line number 325!</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/ScaledInflows.csv</t>
-  </si>
-  <si>
-    <t>Price of Transmission</t>
-  </si>
-  <si>
-    <t>Price related to the usage of tranmission lines (in €/MWh)</t>
-  </si>
-  <si>
-    <t>Reserves Down</t>
-  </si>
-  <si>
-    <t>Reserves Up</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/Reserve2U.csv</t>
-  </si>
-  <si>
-    <t>Price of Unserved H2</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/H2Demand.csv</t>
-  </si>
-  <si>
-    <t>Geo Data</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/Geo_Coordinates.csv</t>
-  </si>
-  <si>
-    <t>Dispa-SET Configuration File (v20.02)</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/H2PtLDemand.csv</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/PtLCapacities.csv</t>
-  </si>
-  <si>
-    <t>H2 Demand (P2H2 - rigid)</t>
-  </si>
-  <si>
-    <t>H2 Demand (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t>H2 Capacities (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/Outages.csv</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/Units_testcase.csv</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/ShareFlex.csv</t>
+    <t>Boundary Sector Supply (flexible)</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_FlexibleSupply.csv</t>
+  </si>
+  <si>
+    <t>CPLEX Accuracy</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Boundary Sector Max Spillage</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Spillage_Capacity.csv</t>
+  </si>
+  <si>
+    <t>Scaled outflows</t>
+  </si>
+  <si>
+    <t>Boundary Sector Reservoir Level</t>
+  </si>
+  <si>
+    <t>Boundary SectorAlert Level</t>
+  </si>
+  <si>
+    <t>Boundary Sector Flood Control</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_AlertLevel.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Flood_control.csv</t>
+  </si>
+  <si>
+    <t>Price of Spillage in the Boundary Sector</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Spillage_cost.csv</t>
+  </si>
+  <si>
+    <t>CPLEX Settings</t>
+  </si>
+  <si>
+    <t>Aggressive</t>
   </si>
 </sst>
 </file>
@@ -748,6 +853,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -768,12 +878,6 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -895,15 +999,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -915,13 +1019,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,11 +1046,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -954,9 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -966,15 +1067,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -988,10 +1080,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1018,17 +1110,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1036,7 +1122,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1049,7 +1135,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1094,15 +1250,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFE9D7A6"/>
-      <color rgb="FFA1A295"/>
-      <color rgb="FFACC0AC"/>
-      <color rgb="FFECBE8B"/>
-      <color rgb="FFD9AE8F"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1115,9 +1262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1155,9 +1302,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1190,26 +1337,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1242,26 +1372,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1438,34 +1551,34 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1478,17 +1591,17 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1501,81 +1614,81 @@
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="A6" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -1586,37 +1699,37 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+    <row r="15" spans="1:8" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="B16" s="25"/>
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B17" s="30"/>
+        <v>176</v>
+      </c>
+      <c r="B17" s="26"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="28"/>
-    </row>
-    <row r="19" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>177</v>
+      </c>
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1630,86 +1743,104 @@
     <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
+    <row r="33" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="32"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>185</v>
+        <v>236</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="4" t="b">
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="4" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>86</v>
+        <v>128</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="39">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
     <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1725,66 +1856,66 @@
     <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
+    <row r="56" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="32"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="28" t="s">
         <v>38</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C57" s="17">
         <v>42005</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C58" s="17">
         <v>42011</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="24" t="s">
         <v>46</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>47</v>
       </c>
       <c r="C59" s="4">
         <v>4</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B60" s="28" t="s">
         <v>47</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="C60" s="4">
         <v>1</v>
@@ -1792,21 +1923,21 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>209</v>
+        <v>197</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>199</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>209</v>
+        <v>198</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>199</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1824,177 +1955,129 @@
     <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
+    <row r="75" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B75" s="32"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
     </row>
     <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="30" t="s">
         <v>60</v>
       </c>
+      <c r="B78" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="C78" s="4" t="s">
-        <v>59</v>
+        <v>212</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="4" t="b">
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="C96" s="1"/>
-    </row>
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="B98" s="36"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="36"/>
+    <row r="98" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" s="32"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>60</v>
+        <v>136</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B100" s="30" t="s">
-        <v>60</v>
+        <v>158</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B101" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B101" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="4" t="b">
@@ -2002,34 +2085,34 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="E102" s="28" t="s">
+      <c r="A102" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E102" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F102" s="5">
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="E103" s="28" t="s">
+      <c r="A103" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E103" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F103" s="5">
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2052,51 +2135,49 @@
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B124" s="36"/>
-      <c r="C124" s="37"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
-      <c r="F124" s="36"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="36"/>
+    <row r="124" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B124" s="32"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="32"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
+      <c r="G124" s="32"/>
+      <c r="H124" s="32"/>
     </row>
     <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="29" t="s">
-        <v>36</v>
+      <c r="B125" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H125" s="11"/>
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B126" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C126" s="19" t="s">
-        <v>233</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B126" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="19"/>
       <c r="D126" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E126" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E126" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F126" s="5">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="H126" s="11"/>
     </row>
@@ -2104,847 +2185,767 @@
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B127" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C127" s="23" t="s">
-        <v>231</v>
-      </c>
+      <c r="B127" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="22"/>
       <c r="D127" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H127" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="29" t="s">
-        <v>36</v>
+      <c r="B128" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B129" s="29" t="s">
         <v>36</v>
       </c>
+      <c r="B129" s="25" t="s">
+        <v>35</v>
+      </c>
       <c r="C129" s="19" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B130" s="29" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="B130" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E130" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E130" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F130" s="5">
         <v>0.05</v>
       </c>
       <c r="H130" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B131" s="29" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="B131" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H131" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B132" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C132" s="19" t="s">
-        <v>189</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B132" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" s="19"/>
       <c r="D132" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H132" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B133" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C133" s="19" t="s">
-        <v>215</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B133" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" s="19"/>
       <c r="D133" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B134" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C134" s="19" t="s">
-        <v>194</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B134" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="19"/>
       <c r="D134" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B135" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C135" s="19" t="s">
-        <v>195</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="B135" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C135" s="19"/>
       <c r="D135" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B136" s="29" t="s">
-        <v>36</v>
+        <v>190</v>
+      </c>
+      <c r="B136" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>200</v>
+        <v>251</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H136" s="11"/>
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B137" s="29" t="s">
-        <v>36</v>
+        <v>245</v>
+      </c>
+      <c r="B137" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B138" s="29" t="s">
-        <v>36</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B138" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="B139" s="29" t="s">
-        <v>36</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B139" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="B140" s="29" t="s">
-        <v>36</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B140" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="25"/>
-      <c r="C141" s="27"/>
-    </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="25"/>
-      <c r="C142" s="27"/>
-    </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="25"/>
-      <c r="C143" s="27"/>
-    </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
-      <c r="C144" s="27"/>
-    </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
-      <c r="C145" s="27"/>
-    </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="25"/>
-      <c r="C146" s="27"/>
-    </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="25"/>
-      <c r="C147" s="27"/>
-    </row>
-    <row r="148" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="25"/>
-      <c r="C148" s="27"/>
-    </row>
-    <row r="149" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="25"/>
-      <c r="C149" s="27"/>
-    </row>
-    <row r="150" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="25"/>
-      <c r="C150" s="27"/>
-    </row>
-    <row r="151" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="25"/>
-      <c r="C151" s="27"/>
-    </row>
-    <row r="152" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="25"/>
-      <c r="C152" s="27"/>
-    </row>
-    <row r="153" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="25"/>
-      <c r="C153" s="27"/>
-    </row>
-    <row r="154" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="25"/>
-      <c r="C154" s="27"/>
-    </row>
-    <row r="155" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="25"/>
-      <c r="C155" s="27"/>
-    </row>
-    <row r="156" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="25"/>
-      <c r="C156" s="27"/>
-    </row>
-    <row r="157" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="25"/>
-      <c r="C157" s="27"/>
-    </row>
-    <row r="158" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="25"/>
-      <c r="C158" s="27"/>
-    </row>
-    <row r="159" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="25"/>
-      <c r="C159" s="27"/>
-    </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="25"/>
-      <c r="C160" s="27"/>
-    </row>
-    <row r="161" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="B161" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C161" s="19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="B162" s="29" t="s">
-        <v>36</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B141" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C141" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B142" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B143" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B144" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B145" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="19"/>
+    </row>
+    <row r="146" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B146" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="19" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B147" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C147" s="19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B161" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C161" s="19"/>
+    </row>
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B162" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C162" s="19"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C163" s="1"/>
-      <c r="E163" s="28" t="s">
+      <c r="E163" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F163" s="5">
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E164" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E164" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F164" s="5">
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="25"/>
-      <c r="C165" s="27"/>
-    </row>
-    <row r="166" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B166" s="36"/>
-      <c r="C166" s="37"/>
-      <c r="D166" s="36"/>
-      <c r="E166" s="36"/>
-      <c r="F166" s="36"/>
-      <c r="G166" s="36"/>
-      <c r="H166" s="36"/>
+    </row>
+    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="B166" s="32"/>
+      <c r="C166" s="33"/>
+      <c r="D166" s="32"/>
+      <c r="E166" s="32"/>
+      <c r="F166" s="32"/>
+      <c r="G166" s="32"/>
+      <c r="H166" s="32"/>
     </row>
     <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B167" s="29" t="s">
-        <v>36</v>
+        <v>121</v>
+      </c>
+      <c r="B167" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C167" s="19"/>
       <c r="D167" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E167" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E167" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F167" s="5">
-        <v>7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B168" s="29" t="s">
-        <v>36</v>
+        <v>141</v>
+      </c>
+      <c r="B168" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C168" s="19"/>
       <c r="D168" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E168" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E168" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B169" s="29" t="s">
-        <v>36</v>
+        <v>134</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C169" s="19"/>
       <c r="D169" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E169" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E169" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F169" s="5">
         <v>400</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B170" s="29" t="s">
-        <v>36</v>
+        <v>205</v>
+      </c>
+      <c r="B170" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C170" s="19"/>
       <c r="D170" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E170" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E170" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F170" s="5">
         <v>0</v>
       </c>
-      <c r="H170" s="26" t="s">
-        <v>217</v>
+      <c r="H170" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B171" s="29" t="s">
-        <v>36</v>
+        <v>246</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C171" s="19"/>
       <c r="D171" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E171" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E171" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="25"/>
-      <c r="C172" s="27"/>
-    </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="25"/>
-      <c r="C173" s="27"/>
-    </row>
-    <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="25"/>
-      <c r="C174" s="27"/>
-    </row>
-    <row r="175" spans="1:8" s="26" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="25"/>
-      <c r="C175" s="27"/>
-    </row>
-    <row r="176" spans="1:8" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="25"/>
-      <c r="C176" s="27"/>
-    </row>
-    <row r="177" spans="1:8" s="26" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="25"/>
-      <c r="C177" s="27"/>
-    </row>
-    <row r="178" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="25"/>
-      <c r="C178" s="27"/>
-    </row>
-    <row r="179" spans="1:8" s="26" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="25"/>
-      <c r="C179" s="27"/>
-    </row>
-    <row r="180" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="25"/>
-      <c r="C180" s="27"/>
-    </row>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F172" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B181" s="29" t="s">
-        <v>36</v>
+        <v>119</v>
+      </c>
+      <c r="B181" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C181" s="19"/>
       <c r="D181" s="18"/>
-      <c r="E181" s="28" t="s">
+      <c r="E181" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F181" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B182" s="29" t="s">
-        <v>36</v>
+        <v>89</v>
+      </c>
+      <c r="B182" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E182" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E182" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F182" s="5">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B183" s="29" t="s">
-        <v>36</v>
+        <v>61</v>
+      </c>
+      <c r="B183" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E183" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E183" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F183" s="5">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B184" s="29" t="s">
-        <v>36</v>
+        <v>62</v>
+      </c>
+      <c r="B184" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E184" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E184" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F184" s="5">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B185" s="29" t="s">
-        <v>36</v>
+        <v>120</v>
+      </c>
+      <c r="B185" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E185" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E185" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F185" s="5">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B186" s="29" t="s">
-        <v>36</v>
+        <v>126</v>
+      </c>
+      <c r="B186" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C186" s="19"/>
       <c r="D186" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E186" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E186" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F186" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B187" s="29" t="s">
-        <v>36</v>
+        <v>127</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E187" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E187" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F187" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="25"/>
-      <c r="C188" s="27"/>
-    </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B188" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C188" s="19"/>
+      <c r="D188" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E188" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>76</v>
+      </c>
+    </row>
     <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="25"/>
-      <c r="C192" s="27"/>
-    </row>
-    <row r="193" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="25"/>
-      <c r="C193" s="27"/>
-    </row>
-    <row r="194" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="25"/>
-      <c r="C194" s="27"/>
-    </row>
-    <row r="195" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="25"/>
-      <c r="C195" s="27"/>
-    </row>
-    <row r="196" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="25"/>
-      <c r="C196" s="27"/>
-    </row>
-    <row r="197" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="25"/>
-      <c r="C197" s="27"/>
-    </row>
-    <row r="198" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="25"/>
-      <c r="C198" s="27"/>
-    </row>
-    <row r="199" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="25"/>
-      <c r="C199" s="27"/>
-    </row>
-    <row r="200" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="25"/>
-      <c r="C200" s="27"/>
-    </row>
-    <row r="201" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="25"/>
-      <c r="C201" s="27"/>
-    </row>
-    <row r="202" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="25"/>
-      <c r="C202" s="27"/>
-    </row>
-    <row r="203" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="25"/>
-      <c r="C203" s="27"/>
-    </row>
-    <row r="204" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="25"/>
-      <c r="C204" s="27"/>
-    </row>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C205" s="1"/>
-      <c r="E205" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F205" s="24">
+      <c r="E205" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F205" s="23">
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C206" s="1"/>
-      <c r="E206" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C206" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E206" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F206" s="5">
         <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C207" s="1"/>
-      <c r="E207" s="28" t="s">
+      <c r="E207" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="25"/>
-      <c r="C209" s="27"/>
-    </row>
-    <row r="210" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="25"/>
-      <c r="C210" s="27"/>
-    </row>
-    <row r="211" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="25"/>
-      <c r="C211" s="27"/>
-    </row>
-    <row r="212" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="25"/>
-      <c r="C212" s="27"/>
-    </row>
-    <row r="213" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="25"/>
-      <c r="C213" s="27"/>
-    </row>
-    <row r="214" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="25"/>
-      <c r="C214" s="27"/>
-    </row>
-    <row r="215" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="25"/>
-      <c r="C215" s="27"/>
-    </row>
-    <row r="216" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="25"/>
-      <c r="C216" s="27"/>
-    </row>
-    <row r="217" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="25"/>
-      <c r="C217" s="27"/>
-    </row>
-    <row r="218" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="25"/>
-      <c r="C218" s="27"/>
-    </row>
-    <row r="219" spans="1:3" s="26" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="25"/>
-      <c r="C219" s="27"/>
-    </row>
-    <row r="220" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="25"/>
-      <c r="C220" s="27"/>
-    </row>
-    <row r="221" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="25"/>
-      <c r="C221" s="27"/>
-    </row>
-    <row r="222" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="25"/>
-      <c r="C222" s="27"/>
-    </row>
-    <row r="223" spans="1:3" s="26" customFormat="1" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="25"/>
-      <c r="C223" s="27"/>
-    </row>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="B225" s="43" t="s">
+    <row r="225" spans="1:8" s="37" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B225" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C225" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="D225" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="E225" s="43" t="s">
+      <c r="C225" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="D225" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E225" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F225" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="G225" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="H225" s="40"/>
+      <c r="F225" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="G225" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="H225" s="36"/>
     </row>
     <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C226" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D226" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E226" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F226" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G226" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B226" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C226" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D226" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E226" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F226" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G226" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="47" t="s">
-        <v>52</v>
-      </c>
       <c r="B227" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2953,29 +2954,29 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F227" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G227" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="41"/>
+      <c r="B228" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D228" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E228" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F227" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G227" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="47"/>
-      <c r="B228" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C228" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D228" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E228" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="F228" s="4" t="b">
         <v>0</v>
       </c>
@@ -2984,9 +2985,9 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="47"/>
+      <c r="A229" s="41"/>
       <c r="B229" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -3005,9 +3006,9 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="47"/>
+      <c r="A230" s="41"/>
       <c r="B230" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -3016,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -3026,7 +3027,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="47"/>
+      <c r="A231" s="41"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F231" s="4" t="b">
         <v>0</v>
@@ -3047,9 +3048,9 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="47"/>
+      <c r="A232" s="41"/>
       <c r="B232" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C232" s="4" t="b">
         <v>0</v>
@@ -3058,7 +3059,7 @@
         <v>0</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
@@ -3068,9 +3069,9 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="47"/>
+      <c r="A233" s="41"/>
       <c r="B233" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C233" s="4" t="b">
         <v>0</v>
@@ -3079,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F233" s="4" t="b">
         <v>0</v>
@@ -3089,7 +3090,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="47"/>
+      <c r="A234" s="41"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3110,7 +3111,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="47"/>
+      <c r="A235" s="41"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3121,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F235" s="4" t="b">
         <v>0</v>
@@ -3131,7 +3132,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="47"/>
+      <c r="A236" s="41"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>0</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F236" s="4" t="b">
         <v>0</v>
@@ -3152,7 +3153,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="47"/>
+      <c r="A237" s="41"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F237" s="4" t="b">
         <v>0</v>
@@ -3173,7 +3174,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="47"/>
+      <c r="A238" s="41"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3184,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F238" s="4" t="b">
         <v>0</v>
@@ -3194,7 +3195,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="47"/>
+      <c r="A239" s="41"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3215,7 +3216,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="47"/>
+      <c r="A240" s="41"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3226,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3236,18 +3237,18 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="47"/>
+      <c r="A241" s="41"/>
       <c r="B241" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D241" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E241" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C241" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D241" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E241" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F241" s="4" t="b">
         <v>0</v>
@@ -3267,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F242" s="4" t="b">
         <v>0</v>
@@ -3287,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F243" s="4" t="b">
         <v>0</v>
@@ -3298,7 +3299,7 @@
     </row>
     <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C244" s="4" t="b">
         <v>0</v>
@@ -3307,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3317,8 +3318,8 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="50" t="s">
-        <v>173</v>
+      <c r="A245" s="44" t="s">
+        <v>168</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3330,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F245" s="4" t="b">
         <v>0</v>
@@ -3340,9 +3341,9 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="50"/>
+      <c r="A246" s="44"/>
       <c r="B246" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3351,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="E246" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F246" s="4" t="b">
         <v>0</v>
@@ -3360,10 +3361,10 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3383,180 +3384,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="25"/>
-      <c r="C248" s="27"/>
-    </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="25"/>
-      <c r="C249" s="27"/>
-    </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="25"/>
-      <c r="C250" s="27"/>
-    </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="25"/>
-      <c r="C251" s="27"/>
-    </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="25"/>
-      <c r="C252" s="27"/>
-    </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="25"/>
-      <c r="C253" s="27"/>
-    </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="25"/>
-      <c r="C254" s="27"/>
-    </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="25"/>
-      <c r="C255" s="27"/>
-    </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="25"/>
-      <c r="C256" s="27"/>
-    </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="25"/>
-      <c r="C257" s="27"/>
-    </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="25"/>
-      <c r="C258" s="27"/>
-    </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="25"/>
-      <c r="C259" s="27"/>
-    </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="25"/>
-      <c r="C260" s="27"/>
-    </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="25"/>
-      <c r="C261" s="27"/>
-    </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="25"/>
-      <c r="C262" s="27"/>
-    </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="25"/>
-      <c r="C263" s="27"/>
-    </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="25"/>
-      <c r="C264" s="27"/>
-    </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="25"/>
-      <c r="C265" s="27"/>
-    </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="25"/>
-      <c r="C266" s="27"/>
-    </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="25"/>
-      <c r="C267" s="27"/>
-    </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="25"/>
-      <c r="C268" s="27"/>
-    </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="25"/>
-      <c r="C269" s="27"/>
-    </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="25"/>
-      <c r="C270" s="27"/>
-    </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="25"/>
-      <c r="C271" s="27"/>
-    </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="25"/>
-      <c r="C272" s="27"/>
-    </row>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B274" s="36"/>
-      <c r="C274" s="37"/>
-      <c r="D274" s="36"/>
-      <c r="E274" s="36"/>
-      <c r="F274" s="36"/>
-      <c r="G274" s="36"/>
-      <c r="H274" s="36"/>
+    <row r="248" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B274" s="32"/>
+      <c r="C274" s="33"/>
+      <c r="D274" s="32"/>
+      <c r="E274" s="32"/>
+      <c r="F274" s="32"/>
+      <c r="G274" s="32"/>
+      <c r="H274" s="32"/>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B275" s="28" t="s">
-        <v>76</v>
+      <c r="B275" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B276" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="B276" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="C276" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H276" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B277" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="B277" s="28" t="s">
-        <v>76</v>
-      </c>
       <c r="C277" s="5">
         <v>1</v>
       </c>
       <c r="H277" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B278" s="28" t="s">
         <v>76</v>
       </c>
+      <c r="B278" s="24" t="s">
+        <v>75</v>
+      </c>
       <c r="C278" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
@@ -3565,158 +3491,319 @@
     <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="301" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="9"/>
-      <c r="C302" s="14"/>
-    </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="304" spans="1:8" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="B304" s="40"/>
-      <c r="C304" s="42"/>
-      <c r="D304" s="40"/>
-      <c r="E304" s="40"/>
-      <c r="F304" s="40"/>
-      <c r="G304" s="40"/>
-      <c r="H304" s="40"/>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A298" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B298" s="32"/>
+      <c r="C298" s="33"/>
+      <c r="D298" s="32"/>
+      <c r="E298" s="32"/>
+      <c r="F298" s="32"/>
+      <c r="G298" s="32"/>
+      <c r="H298" s="32"/>
+    </row>
+    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C299" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D299" s="37"/>
+      <c r="E299" s="37"/>
+      <c r="F299" s="37"/>
+      <c r="G299" s="37"/>
+      <c r="H299" s="37"/>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B300" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C300" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B301" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C301" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B302" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C302" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B303" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C303" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" s="37" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="2"/>
+      <c r="B304" s="1"/>
+      <c r="C304" s="13"/>
+      <c r="D304" s="1"/>
+      <c r="E304" s="1"/>
+      <c r="F304" s="1"/>
+      <c r="G304" s="1"/>
+      <c r="H304" s="1"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C305" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C305" s="27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B306" s="22" t="s">
+      <c r="F305" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B306" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C306" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E306" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F306" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B307" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C307" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E307" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F307" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B308" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C306" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B307" s="22" t="s">
+      <c r="C308" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E308" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F308" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B309" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C307" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B308" s="22" t="s">
+      <c r="C309" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E309" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F309" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B310" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C308" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B309" s="22" t="s">
+      <c r="C310" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E310" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="F310" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B311" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C309" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B310" s="22" t="s">
+      <c r="C311" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E311" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="F311" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B312" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C310" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B311" s="22" t="s">
+      <c r="C312" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E312" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F312" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B313" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C311" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B312" s="22" t="s">
+      <c r="C313" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E313" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F313" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B314" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C312" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B313" s="22" t="s">
+      <c r="C314" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E314" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F314" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B315" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C313" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="22" t="s">
+      <c r="C315" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E315" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="F315" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B316" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C314" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B315" s="22" t="s">
+      <c r="C316" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E316" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F316" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B317" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C315" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B316" s="22" t="s">
+      <c r="C317" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E317" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F317" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B318" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C316" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B317" s="22" t="s">
+      <c r="C318" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E318" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F318" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B319" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C317" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B318" s="22" t="s">
+      <c r="C319" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E319" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="F319" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B320" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C318" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B319" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C319" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B320" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C320" s="21" t="b">
+      <c r="C320" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E320" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="F320" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B321" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C321" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F321" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E322" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F322" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3730,21 +3817,61 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="A245:A246"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 F226:G247 C79 C306:C320 C35:C36">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C35:C36 C79">
+    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="13" priority="25" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="26" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C300:C303">
+    <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C306:C321">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C226:D247">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C226)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F306:F322">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F226:G247">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="547" yWindow="733" count="35">
@@ -3758,102 +3885,84 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F187 F171" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F188 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C37" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F171" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C60 C62" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Look Ahead Period" prompt="This is the overlap period between consecutive optimization of the rolling horizon._x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C60 C62" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>0</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C59 C61" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Horizon length" prompt="This is the number of days to be optimized in the rolling horizon framework. Does not include the overlap period with the next optimization horizon. _x000a__x000a_If HorizonLength is 3 and  LookAhead is 1, optimization length is 4 days, discarding 1 day each time" sqref="C59 C61" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>1</formula1>
       <formula2>365</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169:F170" xr:uid="{1195FB7B-37A6-4912-A3EE-96C2F97F346B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205" xr:uid="{A011503E-FACE-460E-BFDF-1701CC622931}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F206" xr:uid="{55DE26F7-FB99-4503-A869-CFB48A9FAFFA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F207" xr:uid="{93C10F4D-B06D-4B18-B580-B5E72EA43594}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F102" xr:uid="{C22C312A-4C0D-465E-AA40-04829D4E1DD5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F103" xr:uid="{70E3A2FC-178F-4589-82CF-31382B011A9B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C136" xr:uid="{DCD0DDF5-CAA3-4B00-8005-5B7C31C37DA9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand input file" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="C126" xr:uid="{C0A91F47-4A7A-4D7C-8BF7-42344234CEB1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand default value" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="F126" xr:uid="{0207F56E-8010-40B0-B53E-04E2603C9864}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F164" xr:uid="{9C9B8F4F-043F-41E7-8848-A40DCB72B3F5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F163" xr:uid="{C47BA5BE-2C24-4654-BEF9-EA5B433BE488}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{F5C6CB55-A203-47FE-96B0-DC9C451014C9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137:C138" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Load Shedding Costs" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F169:F170" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Value of Lost Load" prompt="Value of Lost Load represents the highest ammount that customers would be willing to pay to avoid disruption. Should be set to a really high value (e.a. &gt;10e5) " sqref="F205" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Price of spillage" prompt="Involuntary water spillage in hydro reservirs. Relativley low value (e.a. &lt;5)" sqref="F206" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Water Value" prompt="Value of water for unsatisfied reservoir levels. High number (e.a. 100 &lt; x &lt; 400)" sqref="F207" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="Initial state of charge. It is defined as the % of total storage capacity." sqref="F102" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max storage)" prompt="FInal state of charge. It is defined as the % of total storage capacity." sqref="F103" xr:uid="{00000000-0002-0000-0000-000015000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hourly temperature data" prompt="Path to the tempeature time series for each zone._x000a_This is required for heating technologies (e.g. temperature-dependent COP)" sqref="C136" xr:uid="{00000000-0002-0000-0000-000016000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand input file" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="C126" xr:uid="{00000000-0002-0000-0000-000017000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible demand default value" prompt="The &quot;Flexible Demand&quot; is the proportion of the demand curve that can be time-shifted (min: 0, max: 1)" sqref="F126" xr:uid="{00000000-0002-0000-0000-000018000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Share of 2U quick start units" prompt="between 0 and 1" sqref="F164" xr:uid="{00000000-0002-0000-0000-000019000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand flexiblity" prompt="Number of hours by which the flexible demand can be shifted" sqref="F163" xr:uid="{00000000-0002-0000-0000-00001A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{00000000-0002-0000-0000-00001B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{00000000-0002-0000-0000-00001C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{00000000-0002-0000-0000-00001D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{00000000-0002-0000-0000-00001E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{00000000-0002-0000-0000-00001F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{00000000-0002-0000-0000-000020000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137" xr:uid="{00000000-0002-0000-0000-000021000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F172" xr:uid="{00000000-0002-0000-0000-000022000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="9">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2208311D-42B6-4F60-9934-B08C9F1E5C51}">
+          <x14:formula1>
+            <xm:f>Lists!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0CD96EF-65E1-4CDC-9807-E214C67B36DE}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C306:C320 F226:G247 C226:D247</xm:sqref>
+          <xm:sqref>C35:C36 C79 C101 C300:C303 C306:C321 F306:F322 F226:G247 C226:D247</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write GDX file" prompt="If set to true, the gdx file is written in the simulation environment directory. Note that the gdx file is required to run the GAMS optimization." xr:uid="{00000000-0002-0000-0000-000013000000}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C35:D35</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write Pickles file" prompt="If set to true, one pickle file (python data format) is written in the simulation environment directory to allow quickly retrieving the simulation inputs" xr:uid="{00000000-0002-0000-0000-000014000000}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C36:D36 D76</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve Calculation" prompt="This inputs allows selecting the metodology for reserve sizing_x000a_" xr:uid="{00000000-0002-0000-0000-000015000000}">
-          <x14:formula1>
-            <xm:f>Lists!$C$2:$C$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>C78</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Allow Curtailment of Renewables" prompt="Set to true to allow curtailment" xr:uid="{00000000-0002-0000-0000-000016000000}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C79</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Simulation type" prompt="Select the type of optimization to perform." xr:uid="{00000000-0002-0000-0000-000017000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{184E1C98-F332-40AF-8944-4EE3B029C322}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>C77</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydro Scheduling" prompt="Select type of mid-term hydro scheduling._x000a_Off: Mid-term scheduling is not performed, hystorical reservoir levels are used instead_x000a_Regional: Performed for the whole region simultaneously_x000a_Zonal: Performed for each zone individually" xr:uid="{86FAD3D9-F1C3-47D5-A81B-4788D9BD562F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5BC13C8-E639-45F1-8901-CB963D4EE0E6}">
           <x14:formula1>
-            <xm:f>Lists!$E$2:$E$6</xm:f>
+            <xm:f>Lists!$C$2:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C78</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A61AE642-9662-46F7-9E7E-D3A7DB5B5708}">
+          <x14:formula1>
+            <xm:f>Lists!$E$2:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>C99</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hydro scheduling horizon" prompt="Annual: Performes hydro scheduling for one year_x000a_Stop-date driven: Performes hydro scheduling between Start and Stop dates_x000a_" xr:uid="{345F7B42-F54C-4808-919E-6CF06ADB107C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{777CC868-04CE-4CC4-896B-21AD7CDCBDEF}">
           <x14:formula1>
-            <xm:f>Lists!$F$2:$F$5</xm:f>
+            <xm:f>Lists!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>C100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Initial/Final reservoir levels" prompt="Values for the initial and final levels, usefull when no reservoir levels are proided as inputs in the Input data" xr:uid="{A38CDE04-BA26-4377-B449-1F28F030BC87}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3864,100 +3973,119 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3977,56 +4105,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" s="20" t="b">
         <v>1</v>
@@ -4073,7 +4201,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="20" t="b">
         <v>1</v>
@@ -4120,7 +4248,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="20" t="b">
         <v>0</v>
@@ -4167,7 +4295,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="20" t="b">
         <v>0</v>
@@ -4214,7 +4342,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="20" t="b">
         <v>1</v>
@@ -4261,7 +4389,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" s="20" t="b">
         <v>1</v>
@@ -4308,7 +4436,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="20" t="b">
         <v>0</v>
@@ -4355,7 +4483,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="20" t="b">
         <v>0</v>
@@ -4402,7 +4530,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B10" s="20" t="b">
         <v>0</v>
@@ -4449,7 +4577,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="20" t="b">
         <v>0</v>
@@ -4496,7 +4624,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B12" s="20" t="b">
         <v>1</v>
@@ -4543,7 +4671,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B13" s="20" t="b">
         <v>1</v>
@@ -4590,7 +4718,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B14" s="20" t="b">
         <v>1</v>
@@ -4637,7 +4765,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B15" s="20" t="b">
         <v>0</v>
@@ -4684,7 +4812,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B16" s="20" t="b">
         <v>0</v>
@@ -4730,9 +4858,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D30">
-    <sortCondition ref="D1"/>
-  </sortState>
   <conditionalFormatting sqref="B2:O16">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
@@ -4742,17 +4867,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:O16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>